<commit_message>
code changed related to failure case
</commit_message>
<xml_diff>
--- a/makaia_framework/data/EditVendor.xlsx
+++ b/makaia_framework/data/EditVendor.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\pointOfSale-workspace\makaia_framework-master\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vchandrakasa\git\Session6_repo\makaia_framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1F2694-8AC5-42A9-A71E-3CBAAA958091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +28,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>verifyEditPopup</t>
-  </si>
-  <si>
-    <t>8220316109</t>
   </si>
   <si>
     <t>Kumar</t>
@@ -46,11 +44,14 @@
   <si>
     <t>VendorNameChanged</t>
   </si>
+  <si>
+    <t>94898883</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,11 +363,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,30 +380,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -411,6 +412,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100767EDDC72BBBD2478DDDC2EF93D9FD02" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c2339c2e5b802fb7f13719667bc84429">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="babdf5ca-2c38-4b41-9b23-4a4d6b11a27f" xmlns:ns4="8cff186d-a7e0-45ea-b789-e61505dbcb46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ecfef231d2b5dd7da392499c94d4b85a" ns3:_="" ns4:_="">
     <xsd:import namespace="babdf5ca-2c38-4b41-9b23-4a4d6b11a27f"/>
@@ -645,15 +655,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -663,6 +664,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4A7D0E8-963A-4755-9C6A-56D18D470C0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F43E90F-22D0-4A94-ADDD-D89C1C0D1533}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -681,14 +690,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4A7D0E8-963A-4755-9C6A-56D18D470C0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2FCB182-281B-4DF0-8855-C00A301FFD65}">
   <ds:schemaRefs>

</xml_diff>